<commit_message>
nlogo tweaks and data from Lindblom run
</commit_message>
<xml_diff>
--- a/badgeNames.xlsx
+++ b/badgeNames.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="18260" yWindow="2360" windowWidth="11980" windowHeight="17000" tabRatio="500"/>
+    <workbookView xWindow="15540" yWindow="0" windowWidth="13360" windowHeight="16900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -154,18 +154,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -182,7 +176,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -527,7 +521,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -535,7 +529,7 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -543,7 +537,7 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -551,7 +545,7 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -559,7 +553,7 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -567,7 +561,7 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -575,7 +569,7 @@
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -583,7 +577,7 @@
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -591,7 +585,7 @@
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -599,7 +593,7 @@
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -607,7 +601,7 @@
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -615,7 +609,7 @@
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -623,7 +617,7 @@
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -631,7 +625,7 @@
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -639,7 +633,7 @@
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -647,7 +641,7 @@
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -655,7 +649,7 @@
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -663,7 +657,7 @@
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -671,20 +665,24 @@
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>35</v>
       </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>